<commit_message>
Altre actualització de la pIa
</commit_message>
<xml_diff>
--- a/graphs/practica_Ia/dades_permanent.xlsx
+++ b/graphs/practica_Ia/dades_permanent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel\UAB\TERCER\LAB Termo\Repositori\graphs\practica_Ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99697086-F2ED-4366-A756-219F137AD37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C2929D-EECA-4217-9026-10248BC7F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-870" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D3_dades_estat_permanent" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>u(t) [s]</t>
+  </si>
+  <si>
+    <t>u(d) [cm]</t>
+  </si>
+  <si>
+    <t>u(T) ºC</t>
+  </si>
+  <si>
+    <t>amplitud gran</t>
+  </si>
+  <si>
+    <t>amplitud petita</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,12 +77,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,10 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,6 +145,2896 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>gran</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$P$1:$R$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$P$3:$R$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>81.848796765682565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.011961536900358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.938155243542496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1EB9-4EE7-A580-A4A987B936B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>petit</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$S$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$S$3:$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>98.716907981549824</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.41991709040586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.485790108856094</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1EB9-4EE7-A580-A4A987B936B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1977909055"/>
+        <c:axId val="1977905215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1977909055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1977905215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1977905215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1977909055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>gran</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.23962662274521068"/>
+                  <c:y val="-0.57387165133456641"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$X$7:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$Y$7:$Y$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2178</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80220000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-23B8-46E1-8A88-D621AC480EFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1113734080"/>
+        <c:axId val="1113736480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1113734080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113736480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1113736480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1113734080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>petita</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.22449931053574312"/>
+                  <c:y val="-0.61668677798141636"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$X$11:$X$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>D3_dades_estat_permanent!$Y$11:$Y$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.4036</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2730999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96099999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-065C-43F2-83A0-8CDD3B99FB7E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1299491888"/>
+        <c:axId val="1299490928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1299491888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1299490928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1299490928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1299491888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>455742</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>131781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>631340</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70EB828C-0368-22B9-4799-946AC3008486}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>401595</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>707081</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>70707</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB775FAD-CB42-65D8-B00C-7118875AC34D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>387865</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>6864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>707081</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>89243</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAA5F19-A10B-4E7D-A836-42BD85E7B553}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,10 +3356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F66A18-617D-4E85-BFD5-5F52539CF5CC}">
-  <dimension ref="A1:V543"/>
+  <dimension ref="A1:Y543"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="R2" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,10 +3369,11 @@
     <col min="3" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>9.173</v>
       </c>
@@ -481,6 +3395,7 @@
       <c r="G2" s="1">
         <v>65.463843999999995</v>
       </c>
+      <c r="H2" s="1"/>
       <c r="I2">
         <f>D3_dades_estat_permanent[[#This Row],[t.gran 0cm]]/$P$3</f>
         <v>0.98169426033259943</v>
@@ -524,7 +3439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>17.797999999999998</v>
       </c>
@@ -546,6 +3461,7 @@
       <c r="G3" s="1">
         <v>65.382110999999995</v>
       </c>
+      <c r="H3" s="1"/>
       <c r="I3">
         <f>D3_dades_estat_permanent[[#This Row],[t.gran 0cm]]/$P$3</f>
         <v>0.98343231887006644</v>
@@ -571,32 +3487,31 @@
         <v>0.98339977449242821</v>
       </c>
       <c r="P3">
-        <f>AVERAGE(B:B)</f>
+        <f t="shared" ref="P3:U3" si="0">AVERAGE(B:B)</f>
         <v>81.848796765682565</v>
       </c>
       <c r="Q3">
-        <f>AVERAGE(C:C)</f>
+        <f t="shared" si="0"/>
         <v>72.011961536900358</v>
       </c>
       <c r="R3">
-        <f>AVERAGE(D:D)</f>
+        <f t="shared" si="0"/>
         <v>67.938155243542496</v>
       </c>
       <c r="S3">
-        <f>AVERAGE(E:E)</f>
+        <f t="shared" si="0"/>
         <v>98.716907981549824</v>
       </c>
       <c r="T3">
-        <f>AVERAGE(F:F)</f>
+        <f t="shared" si="0"/>
         <v>80.41991709040586</v>
       </c>
       <c r="U3">
-        <f>AVERAGE(G:G)</f>
+        <f t="shared" si="0"/>
         <v>66.485790108856094</v>
       </c>
-      <c r="V3" s="2"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>26.222000000000001</v>
       </c>
@@ -618,6 +3533,7 @@
       <c r="G4" s="1">
         <v>65.316483000000005</v>
       </c>
+      <c r="H4" s="1"/>
       <c r="I4">
         <f>D3_dades_estat_permanent[[#This Row],[t.gran 0cm]]/$P$3</f>
         <v>0.98594908158546379</v>
@@ -643,7 +3559,7 @@
         <v>0.98241267634871154</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>34.646999999999998</v>
       </c>
@@ -690,7 +3606,7 @@
         <v>0.98201138759277862</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43.073</v>
       </c>
@@ -736,8 +3652,11 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.98090127068089172</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>51.497999999999998</v>
       </c>
@@ -783,8 +3702,23 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.98089277262440344</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>59.920999999999999</v>
       </c>
@@ -830,8 +3764,23 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.98043377228839146</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>1E-3</v>
+      </c>
+      <c r="Q8">
+        <v>0.5</v>
+      </c>
+      <c r="R8">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8">
+        <v>1.2178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>68.344999999999999</v>
       </c>
@@ -877,8 +3826,14 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.9797914997075875</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X9">
+        <v>15</v>
+      </c>
+      <c r="Y9">
+        <v>0.80220000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>76.77</v>
       </c>
@@ -924,8 +3879,11 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.97997923907233853</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>85.195999999999998</v>
       </c>
@@ -971,8 +3929,14 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.97923265848844632</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>5.4036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>93.619</v>
       </c>
@@ -1018,8 +3982,14 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.97971989042096841</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X12">
+        <v>10</v>
+      </c>
+      <c r="Y12">
+        <v>2.2730999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>102.04300000000001</v>
       </c>
@@ -1065,8 +4035,14 @@
         <f>D3_dades_estat_permanent[[#This Row],[t.petita 20cm]]/$U$3</f>
         <v>0.97984221731197307</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X13">
+        <v>20</v>
+      </c>
+      <c r="Y13">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>110.468</v>
       </c>
@@ -1113,7 +4089,7 @@
         <v>0.98036320081752049</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>118.89100000000001</v>
       </c>
@@ -1160,7 +4136,7 @@
         <v>0.98074210885123347</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>127.31399999999999</v>
       </c>
@@ -1631,10 +4607,10 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>211.55099999999999</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>84.421111999999994</v>
       </c>
       <c r="C26" s="1">
@@ -5297,10 +8273,10 @@
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="A104" s="3">
         <v>868.60199999999998</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="3">
         <v>84.505050999999995</v>
       </c>
       <c r="C104">
@@ -25979,8 +28955,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>